<commit_message>
fix: update course content template file
</commit_message>
<xml_diff>
--- a/server/public/templates/course_content_template.xlsx
+++ b/server/public/templates/course_content_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nasty\Downloads\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\task-reminder\app\server\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEB9005-0B5D-46CC-ACD3-C68209EE3A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9277B4A-68F0-4E39-AFCE-DE3D6AA886D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{72780285-2AC5-4CB5-8961-C76F955F97FD}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Semester 14</t>
-  </si>
-  <si>
     <t>COURSE314</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Hour End</t>
+  </si>
+  <si>
+    <t>Semester 1</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,54 +451,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>